<commit_message>
adding new progress as of date 04 nov 2025
</commit_message>
<xml_diff>
--- a/Employee_Reports35/AbdulRashid Byarugaba Q0589.xlsx
+++ b/Employee_Reports35/AbdulRashid Byarugaba Q0589.xlsx
@@ -563,11 +563,11 @@
         </is>
       </c>
       <c r="H3" s="3" t="n">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J3" s="3" t="inlineStr">
@@ -612,11 +612,11 @@
         </is>
       </c>
       <c r="H4" s="3" t="n">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J4" s="3" t="inlineStr">
@@ -661,11 +661,11 @@
         </is>
       </c>
       <c r="H5" s="3" t="n">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I5" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J5" s="3" t="inlineStr">
@@ -710,11 +710,11 @@
         </is>
       </c>
       <c r="H6" s="3" t="n">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I6" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J6" s="3" t="inlineStr">
@@ -759,11 +759,11 @@
         </is>
       </c>
       <c r="H7" s="3" t="n">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I7" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J7" s="3" t="inlineStr">
@@ -808,11 +808,11 @@
         </is>
       </c>
       <c r="H8" s="3" t="n">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I8" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J8" s="3" t="inlineStr">
@@ -857,11 +857,11 @@
         </is>
       </c>
       <c r="H9" s="3" t="n">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I9" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J9" s="3" t="inlineStr">
@@ -906,11 +906,11 @@
         </is>
       </c>
       <c r="H10" s="3" t="n">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I10" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J10" s="3" t="inlineStr">
@@ -955,11 +955,11 @@
         </is>
       </c>
       <c r="H11" s="3" t="n">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I11" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J11" s="3" t="inlineStr">
@@ -1004,11 +1004,11 @@
         </is>
       </c>
       <c r="H12" s="3" t="n">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I12" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J12" s="3" t="inlineStr">
@@ -1053,11 +1053,11 @@
         </is>
       </c>
       <c r="H13" s="3" t="n">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I13" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J13" s="3" t="inlineStr">
@@ -1102,11 +1102,11 @@
         </is>
       </c>
       <c r="H14" s="3" t="n">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I14" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J14" s="3" t="inlineStr">
@@ -1151,11 +1151,11 @@
         </is>
       </c>
       <c r="H15" s="3" t="n">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J15" s="3" t="inlineStr">
@@ -1201,11 +1201,11 @@
         </is>
       </c>
       <c r="H16" s="3" t="n">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J16" s="3" t="inlineStr">
@@ -1250,11 +1250,11 @@
         </is>
       </c>
       <c r="H17" s="3" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J17" s="3" t="inlineStr">
@@ -1299,11 +1299,11 @@
         </is>
       </c>
       <c r="H18" s="3" t="n">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J18" s="3" t="inlineStr">
@@ -1348,11 +1348,11 @@
         </is>
       </c>
       <c r="H19" s="3" t="n">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr">
@@ -1397,11 +1397,11 @@
         </is>
       </c>
       <c r="H20" s="3" t="n">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J20" s="3" t="inlineStr">
@@ -1446,11 +1446,11 @@
         </is>
       </c>
       <c r="H21" s="3" t="n">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I21" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J21" s="3" t="inlineStr">
@@ -1483,11 +1483,11 @@
         </is>
       </c>
       <c r="H22" s="3" t="n">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J22" s="3" t="inlineStr">
@@ -1520,11 +1520,11 @@
         </is>
       </c>
       <c r="H23" s="3" t="n">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I23" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J23" s="3" t="inlineStr">
@@ -1557,11 +1557,11 @@
         </is>
       </c>
       <c r="H24" s="3" t="n">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I24" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J24" s="3" t="inlineStr">
@@ -1594,11 +1594,11 @@
         </is>
       </c>
       <c r="H25" s="3" t="n">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I25" s="3" t="inlineStr">
         <is>
-          <t>03-Nov-2025</t>
+          <t>04-Nov-2025</t>
         </is>
       </c>
       <c r="J25" s="3" t="inlineStr">

</xml_diff>